<commit_message>
product add typename item
</commit_message>
<xml_diff>
--- a/script/http_cmd.xlsx
+++ b/script/http_cmd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="777" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="777" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="http报文样例" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4015" uniqueCount="1555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4025" uniqueCount="1560">
   <si>
     <t>列8</t>
   </si>
@@ -7720,74 +7720,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{
- "retcode":"0",
- "retmsg":"Ok",
- "pdtid":"wioio",
- "name":"xxx",
- "type":"0",
- "aliasname":"mmm",
- "price":"90",
- "pic":"http://xx",
- "extend":"mmm",
- "property":[
-    {"pdtpptid":"wuuu","p_type":"0", "p_name":"xxx", "p_value":"70"},
-    {"pdtpptid":"wuuu","p_type":"1", "p_name":"yyy", "p_value":"wwm"}
-  ]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- "retcode": "0",
- "retmsg": "Ok",
- "product_info": [{
-   "name": "xxx",
-   "pdtid": "wioio",
-   "type": "0",
-   "aliasname": "mmm",
-   "price": "90",
-   "pic": "http://xx",
-   "extend": "mmm",
-   "property": [{
-     "pdtpptid": "wuuu",
-     "p_type": "0",
-     "p_name": "xxx",
-     "p_value": "70"
-    },
-    {
-     "pdtpptid": "wuuu",
-     "p_type": "1",
-     "p_name": "yyy",
-     "p_value": "wwm"
-    }]
-  },
-  {
-   "name": "xxx",
-   "pdtid": "zzzz",
-   "type": "1",
-   "aliasname": "www",
-   "price": "90",
-   "pic": "http://xx",
-   "extend": "mmm",
-   "property": [{
-     "pdtpptid": "wuuu",
-     "p_type": "0",
-     "p_name": "xxx",
-     "p_value": "70"
-    },
-    {
-     "pdtpptid": "wuuu",
-     "p_type": "1",
-     "p_name": "yyy",
-     "p_value": "wwm"
-    }]
-  }
- ]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7983,6 +7915,97 @@
   <si>
     <t>若为空，
 则删除所有订单详情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0：巡店业务类型，1：产品订单管理业务类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备登陆</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备登陆被拒绝</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型名称信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "retcode":"0",
+ "retmsg":"Ok",
+ "pdtid":"wioio",
+ "name":"xxx",
+ "type":"0",
+ "type_name":"ipc",
+ "aliasname":"mmm",
+ "price":"90",
+ "pic":"http://xx",
+ "extend":"mmm",
+ "property":[
+    {"pdtpptid":"wuuu","p_type":"0", "p_name":"xxx", "p_value":"70"},
+    {"pdtpptid":"wuuu","p_type":"1", "p_name":"yyy", "p_value":"wwm"}
+  ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "retcode": "0",
+ "retmsg": "Ok",
+ "product_info": [{
+   "name": "xxx",
+   "pdtid": "wioio",
+   "type": "0",
+   "type_name":"ipc",
+   "aliasname": "mmm",
+   "price": "90",
+   "pic": "http://xx",
+   "extend": "mmm",
+   "property": [{
+     "pdtpptid": "wuuu",
+     "p_type": "0",
+     "p_name": "xxx",
+     "p_value": "70"
+    },
+    {
+     "pdtpptid": "wuuu",
+     "p_type": "1",
+     "p_name": "yyy",
+     "p_value": "wwm"
+    }]
+  },
+  {
+   "name": "xxx",
+   "pdtid": "zzzz",
+   "type": "1",
+   "type_name":"dvr",
+   "aliasname": "www",
+   "price": "90",
+   "pic": "http://xx",
+   "extend": "mmm",
+   "property": [{
+     "pdtpptid": "wuuu",
+     "p_type": "0",
+     "p_name": "xxx",
+     "p_value": "70"
+    },
+    {
+     "pdtpptid": "wuuu",
+     "p_type": "1",
+     "p_name": "yyy",
+     "p_value": "wwm"
+    }]
+  }
+ ]
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11435,8 +11458,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="表1_8" displayName="表1_8" ref="A1:M115" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:M115"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="表1_8" displayName="表1_8" ref="A1:M117" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:M117"/>
   <tableColumns count="13">
     <tableColumn id="1" name="命令名称" dataDxfId="27"/>
     <tableColumn id="13" name="命令类型" dataDxfId="26"/>
@@ -13790,11 +13813,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M130"/>
+  <dimension ref="A1:M132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -13922,7 +13945,7 @@
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="E5" s="9" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>102</v>
@@ -13940,77 +13963,84 @@
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="137"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="9" t="s">
+        <v>1557</v>
+      </c>
       <c r="F6" s="9" t="s">
-        <v>1449</v>
+        <v>1556</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="9">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="M6" s="14"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="139"/>
+      <c r="L6" s="139"/>
+      <c r="M6" s="141"/>
     </row>
     <row r="7" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="9" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="F7" s="9" t="s">
+        <v>1449</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="9">
+        <v>32</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A8" s="102"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="9" t="s">
         <v>1462</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F8" s="104" t="s">
         <v>1459</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>1460</v>
       </c>
-      <c r="H7" s="104">
+      <c r="H8" s="104">
         <v>64</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>1461</v>
       </c>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="106"/>
-    </row>
-    <row r="8" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="F8" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="9">
-        <v>32</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" s="9"/>
-      <c r="M8" s="14"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="106"/>
     </row>
     <row r="9" spans="1:13" ht="31.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="F9" s="9" t="s">
-        <v>570</v>
+        <v>115</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H9" s="9">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>110</v>
@@ -14021,60 +14051,60 @@
     <row r="10" spans="1:13" ht="31.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
+      <c r="F10" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="9">
+        <v>200</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="J10" s="9"/>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:13" ht="54">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="J11" s="9"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" ht="54">
+      <c r="A12" s="8" t="s">
         <v>1451</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>1452</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="9">
-        <v>32</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="9">
+        <v>32</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" ht="31.5" customHeight="1">
-      <c r="F12" s="9" t="s">
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" ht="31.5" customHeight="1">
+      <c r="F13" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="9">
-        <v>32</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" ht="31.5" customHeight="1">
-      <c r="E13" s="12" t="s">
-        <v>1454</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>1453</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>12</v>
@@ -14088,53 +14118,53 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1">
+      <c r="E14" s="12" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="9">
+        <v>32</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="54">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:13" ht="31.5" customHeight="1">
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" ht="54">
+      <c r="A16" s="10" t="s">
         <v>1455</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>1456</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="9">
-        <v>32</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="G16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="9">
+        <v>32</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="J15" s="9"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="F16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="9">
-        <v>32</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="J16" s="9"/>
       <c r="M16" s="14"/>
@@ -14142,11 +14172,8 @@
     <row r="17" spans="1:13" ht="31.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
-      <c r="E17" s="12" t="s">
-        <v>1454</v>
-      </c>
       <c r="F17" s="9" t="s">
-        <v>1453</v>
+        <v>25</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>12</v>
@@ -14163,8 +14190,11 @@
     <row r="18" spans="1:13" ht="31.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
+      <c r="E18" s="12" t="s">
+        <v>1454</v>
+      </c>
       <c r="F18" s="9" t="s">
-        <v>1448</v>
+        <v>1453</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>12</v>
@@ -14173,7 +14203,7 @@
         <v>32</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="J18" s="9"/>
       <c r="M18" s="14"/>
@@ -14182,7 +14212,7 @@
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="F19" s="9" t="s">
-        <v>102</v>
+        <v>1448</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>12</v>
@@ -14200,7 +14230,7 @@
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="F20" s="9" t="s">
-        <v>1449</v>
+        <v>102</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>12</v>
@@ -14218,10 +14248,10 @@
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="E21" s="9" t="s">
-        <v>1464</v>
+        <v>1557</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>1459</v>
+        <v>1556</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>12</v>
@@ -14230,7 +14260,7 @@
         <v>64</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1463</v>
+        <v>17</v>
       </c>
       <c r="J21" s="9"/>
       <c r="M21" s="14"/>
@@ -14239,7 +14269,7 @@
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="F22" s="9" t="s">
-        <v>115</v>
+        <v>1449</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>12</v>
@@ -14256,17 +14286,20 @@
     <row r="23" spans="1:13" ht="31.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
+      <c r="E23" s="9" t="s">
+        <v>1464</v>
+      </c>
       <c r="F23" s="9" t="s">
-        <v>570</v>
+        <v>1459</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H23" s="9">
-        <v>200</v>
+        <v>64</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>110</v>
+        <v>1463</v>
       </c>
       <c r="J23" s="9"/>
       <c r="M23" s="14"/>
@@ -14274,36 +14307,35 @@
     <row r="24" spans="1:13" ht="31.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
+      <c r="F24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="9">
+        <v>32</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="J24" s="9"/>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" spans="1:13" ht="229.5">
-      <c r="A25" s="10" t="s">
-        <v>1467</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>1519</v>
-      </c>
+    <row r="25" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
       <c r="F25" s="9" t="s">
-        <v>28</v>
+        <v>570</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="H25" s="9">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="J25" s="9"/>
       <c r="M25" s="14"/>
@@ -14311,29 +14343,27 @@
     <row r="26" spans="1:13" ht="31.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
-      <c r="F26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="9">
-        <v>32</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J26" s="9"/>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="E27" s="12" t="s">
-        <v>1454</v>
+    <row r="27" spans="1:13" ht="243">
+      <c r="A27" s="10" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>1558</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>1453</v>
+        <v>28</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>12</v>
@@ -14350,28 +14380,29 @@
     <row r="28" spans="1:13" ht="31.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
-      <c r="E28" s="12"/>
+      <c r="F28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="9">
+        <v>32</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="J28" s="9"/>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="1:13" ht="409.5">
-      <c r="A29" s="10" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>1471</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>1520</v>
+    <row r="29" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="E29" s="12" t="s">
+        <v>1454</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>28</v>
+        <v>1453</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>12</v>
@@ -14389,45 +14420,46 @@
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="9">
-        <v>32</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J30" s="9"/>
       <c r="M30" s="14"/>
     </row>
-    <row r="31" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
+    <row r="31" spans="1:13" ht="409.5">
+      <c r="A31" s="10" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>1559</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="9">
+        <v>32</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="J31" s="9"/>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="1:13" ht="67.5">
-      <c r="A32" s="10" t="s">
-        <v>1457</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>1458</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>1526</v>
-      </c>
+    <row r="32" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -14436,7 +14468,7 @@
         <v>32</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="J32" s="9"/>
       <c r="M32" s="14"/>
@@ -14444,29 +14476,27 @@
     <row r="33" spans="1:13" ht="31.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
-      <c r="F33" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="9">
-        <v>32</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J33" s="9"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="E34" s="9" t="s">
-        <v>1454</v>
+    <row r="34" spans="1:13" ht="67.5">
+      <c r="A34" s="10" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>1524</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>1453</v>
+        <v>28</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -14475,25 +14505,22 @@
         <v>32</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="J34" s="9"/>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="1:13" ht="27">
+    <row r="35" spans="1:13" ht="31.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
-      <c r="E35" s="12" t="s">
-        <v>1527</v>
-      </c>
       <c r="F35" s="9" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H35" s="9">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>13</v>
@@ -14501,69 +14528,65 @@
       <c r="J35" s="9"/>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A36" s="137"/>
-      <c r="B36" s="138"/>
-      <c r="C36" s="139"/>
-      <c r="D36" s="140"/>
-      <c r="E36" s="140"/>
+    <row r="36" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="E36" s="9" t="s">
+        <v>1454</v>
+      </c>
       <c r="F36" s="9" t="s">
-        <v>1521</v>
+        <v>1453</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H36" s="139">
+        <v>12</v>
+      </c>
+      <c r="H36" s="9">
         <v>32</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>1522</v>
-      </c>
-      <c r="J36" s="139"/>
-      <c r="K36" s="139"/>
-      <c r="L36" s="139"/>
-      <c r="M36" s="141"/>
-    </row>
-    <row r="37" spans="1:13" ht="38.25" customHeight="1">
-      <c r="A37" s="137"/>
-      <c r="B37" s="138"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="140"/>
-      <c r="E37" s="140"/>
+        <v>13</v>
+      </c>
+      <c r="J36" s="9"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:13" ht="27">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="E37" s="12" t="s">
+        <v>1525</v>
+      </c>
       <c r="F37" s="9" t="s">
-        <v>1523</v>
+        <v>102</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>1524</v>
-      </c>
-      <c r="H37" s="139">
-        <v>300</v>
+        <v>12</v>
+      </c>
+      <c r="H37" s="9">
+        <v>2</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>1525</v>
-      </c>
-      <c r="J37" s="139"/>
-      <c r="K37" s="139"/>
-      <c r="L37" s="139"/>
-      <c r="M37" s="141"/>
-    </row>
-    <row r="38" spans="1:13" ht="38.25" customHeight="1">
+        <v>13</v>
+      </c>
+      <c r="J37" s="9"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" ht="30.75" customHeight="1">
       <c r="A38" s="137"/>
       <c r="B38" s="138"/>
       <c r="C38" s="139"/>
       <c r="D38" s="140"/>
       <c r="E38" s="140"/>
-      <c r="F38" s="139" t="s">
-        <v>570</v>
+      <c r="F38" s="9" t="s">
+        <v>1519</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>113</v>
       </c>
       <c r="H38" s="139">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>110</v>
+        <v>1520</v>
       </c>
       <c r="J38" s="139"/>
       <c r="K38" s="139"/>
@@ -14576,79 +14599,86 @@
       <c r="C39" s="139"/>
       <c r="D39" s="140"/>
       <c r="E39" s="140"/>
-      <c r="F39" s="139"/>
-      <c r="G39" s="139"/>
-      <c r="H39" s="139"/>
-      <c r="I39" s="139"/>
+      <c r="F39" s="9" t="s">
+        <v>1521</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>1522</v>
+      </c>
+      <c r="H39" s="139">
+        <v>300</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>1523</v>
+      </c>
       <c r="J39" s="139"/>
       <c r="K39" s="139"/>
       <c r="L39" s="139"/>
       <c r="M39" s="141"/>
     </row>
-    <row r="40" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="E40" s="12"/>
-      <c r="J40" s="9"/>
-      <c r="M40" s="14"/>
-    </row>
-    <row r="41" spans="1:13" ht="54">
-      <c r="A41" s="10" t="s">
-        <v>1465</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>1466</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="9">
-        <v>32</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J41" s="9"/>
-      <c r="M41" s="14"/>
-    </row>
-    <row r="42" spans="1:13" ht="31.5" customHeight="1">
+    <row r="40" spans="1:13" ht="38.25" customHeight="1">
+      <c r="A40" s="137"/>
+      <c r="B40" s="138"/>
+      <c r="C40" s="139"/>
+      <c r="D40" s="140"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="139" t="s">
+        <v>570</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H40" s="139">
+        <v>300</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J40" s="139"/>
+      <c r="K40" s="139"/>
+      <c r="L40" s="139"/>
+      <c r="M40" s="141"/>
+    </row>
+    <row r="41" spans="1:13" ht="38.25" customHeight="1">
+      <c r="A41" s="137"/>
+      <c r="B41" s="138"/>
+      <c r="C41" s="139"/>
+      <c r="D41" s="140"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="139"/>
+      <c r="G41" s="139"/>
+      <c r="H41" s="139"/>
+      <c r="I41" s="139"/>
+      <c r="J41" s="139"/>
+      <c r="K41" s="139"/>
+      <c r="L41" s="139"/>
+      <c r="M41" s="141"/>
+    </row>
+    <row r="42" spans="1:13" ht="30.75" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
-      <c r="F42" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="9">
-        <v>32</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="E42" s="12"/>
       <c r="J42" s="9"/>
       <c r="M42" s="14"/>
     </row>
-    <row r="43" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="E43" s="9" t="s">
-        <v>1454</v>
+    <row r="43" spans="1:13" ht="54">
+      <c r="A43" s="10" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>1453</v>
+        <v>28</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>12</v>
@@ -14665,14 +14695,8 @@
     <row r="44" spans="1:13" ht="31.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
-      <c r="D44" s="12" t="s">
-        <v>1518</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>1470</v>
-      </c>
       <c r="F44" s="9" t="s">
-        <v>1469</v>
+        <v>25</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>12</v>
@@ -14681,7 +14705,7 @@
         <v>32</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="J44" s="9"/>
       <c r="M44" s="14"/>
@@ -14689,27 +14713,35 @@
     <row r="45" spans="1:13" ht="31.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
+      <c r="E45" s="9" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="9">
+        <v>32</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="J45" s="9"/>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="1:13" ht="67.5">
-      <c r="A46" s="10" t="s">
-        <v>1473</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>1474</v>
-      </c>
+    <row r="46" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
       <c r="D46" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>1475</v>
+        <v>1518</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>1470</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>28</v>
+        <v>1469</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>12</v>
@@ -14718,7 +14750,7 @@
         <v>32</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="J46" s="9"/>
       <c r="M46" s="14"/>
@@ -14726,29 +14758,27 @@
     <row r="47" spans="1:13" ht="31.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
-      <c r="F47" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="9">
-        <v>32</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J47" s="9"/>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
-      <c r="E48" s="9" t="s">
-        <v>1550</v>
-      </c>
-      <c r="F48" s="139" t="s">
-        <v>1549</v>
+    <row r="48" spans="1:13" ht="67.5">
+      <c r="A48" s="10" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>12</v>
@@ -14765,20 +14795,17 @@
     <row r="49" spans="1:13" ht="31.5" customHeight="1">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
-      <c r="E49" s="9" t="s">
-        <v>1481</v>
-      </c>
       <c r="F49" s="9" t="s">
-        <v>1476</v>
+        <v>25</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>1477</v>
+        <v>12</v>
       </c>
       <c r="H49" s="9">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>1478</v>
+        <v>13</v>
       </c>
       <c r="J49" s="9"/>
       <c r="M49" s="14"/>
@@ -14787,19 +14814,19 @@
       <c r="A50" s="10"/>
       <c r="B50" s="11"/>
       <c r="E50" s="9" t="s">
-        <v>1480</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>1479</v>
+        <v>1548</v>
+      </c>
+      <c r="F50" s="139" t="s">
+        <v>1547</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H50" s="9">
         <v>32</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>1478</v>
+        <v>13</v>
       </c>
       <c r="J50" s="9"/>
       <c r="M50" s="14"/>
@@ -14808,19 +14835,19 @@
       <c r="A51" s="10"/>
       <c r="B51" s="11"/>
       <c r="E51" s="9" t="s">
-        <v>1496</v>
+        <v>1481</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>1497</v>
+        <v>1476</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>16</v>
+        <v>1477</v>
       </c>
       <c r="H51" s="9">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>1498</v>
+        <v>1478</v>
       </c>
       <c r="J51" s="9"/>
       <c r="M51" s="14"/>
@@ -14828,11 +14855,11 @@
     <row r="52" spans="1:13" ht="31.5" customHeight="1">
       <c r="A52" s="10"/>
       <c r="B52" s="11"/>
-      <c r="E52" s="12" t="s">
-        <v>1482</v>
+      <c r="E52" s="9" t="s">
+        <v>1480</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>1508</v>
+        <v>1479</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>16</v>
@@ -14841,7 +14868,7 @@
         <v>32</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>17</v>
+        <v>1478</v>
       </c>
       <c r="J52" s="9"/>
       <c r="M52" s="14"/>
@@ -14850,19 +14877,19 @@
       <c r="A53" s="10"/>
       <c r="B53" s="11"/>
       <c r="E53" s="9" t="s">
-        <v>1484</v>
+        <v>1496</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>1483</v>
+        <v>1497</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>1477</v>
+        <v>16</v>
       </c>
       <c r="H53" s="9">
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>1478</v>
+        <v>1498</v>
       </c>
       <c r="J53" s="9"/>
       <c r="M53" s="14"/>
@@ -14870,20 +14897,20 @@
     <row r="54" spans="1:13" ht="31.5" customHeight="1">
       <c r="A54" s="10"/>
       <c r="B54" s="11"/>
-      <c r="E54" s="9" t="s">
-        <v>1486</v>
+      <c r="E54" s="12" t="s">
+        <v>1482</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>1485</v>
+        <v>1508</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>1477</v>
+        <v>16</v>
       </c>
       <c r="H54" s="9">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>1478</v>
+        <v>17</v>
       </c>
       <c r="J54" s="9"/>
       <c r="M54" s="14"/>
@@ -14892,19 +14919,19 @@
       <c r="A55" s="10"/>
       <c r="B55" s="11"/>
       <c r="E55" s="9" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>1489</v>
+        <v>1477</v>
       </c>
       <c r="H55" s="9">
-        <v>64</v>
+        <v>500</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>1490</v>
+        <v>1478</v>
       </c>
       <c r="J55" s="9"/>
       <c r="M55" s="14"/>
@@ -14913,19 +14940,19 @@
       <c r="A56" s="10"/>
       <c r="B56" s="11"/>
       <c r="E56" s="9" t="s">
-        <v>1492</v>
+        <v>1486</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>1491</v>
+        <v>1485</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>1489</v>
+        <v>1477</v>
       </c>
       <c r="H56" s="9">
-        <v>64</v>
+        <v>200</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>1490</v>
+        <v>1478</v>
       </c>
       <c r="J56" s="9"/>
       <c r="M56" s="14"/>
@@ -14934,19 +14961,19 @@
       <c r="A57" s="10"/>
       <c r="B57" s="11"/>
       <c r="E57" s="9" t="s">
-        <v>1495</v>
+        <v>1487</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>1493</v>
+        <v>1488</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>1477</v>
+        <v>1489</v>
       </c>
       <c r="H57" s="9">
-        <v>200</v>
+        <v>64</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
       <c r="J57" s="9"/>
       <c r="M57" s="14"/>
@@ -14954,36 +14981,41 @@
     <row r="58" spans="1:13" ht="31.5" customHeight="1">
       <c r="A58" s="10"/>
       <c r="B58" s="11"/>
+      <c r="E58" s="9" t="s">
+        <v>1492</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H58" s="9">
+        <v>64</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>1490</v>
+      </c>
       <c r="J58" s="9"/>
       <c r="M58" s="14"/>
     </row>
-    <row r="59" spans="1:13" ht="67.5">
-      <c r="A59" s="10" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>1546</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>1534</v>
+    <row r="59" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A59" s="10"/>
+      <c r="B59" s="11"/>
+      <c r="E59" s="9" t="s">
+        <v>1495</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>28</v>
+        <v>1493</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>12</v>
+        <v>1477</v>
       </c>
       <c r="H59" s="9">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>13</v>
+        <v>1494</v>
       </c>
       <c r="J59" s="9"/>
       <c r="M59" s="14"/>
@@ -14991,29 +15023,27 @@
     <row r="60" spans="1:13" ht="31.5" customHeight="1">
       <c r="A60" s="10"/>
       <c r="B60" s="11"/>
-      <c r="F60" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" s="9">
-        <v>32</v>
-      </c>
-      <c r="I60" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J60" s="9"/>
       <c r="M60" s="14"/>
     </row>
-    <row r="61" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="E61" s="9" t="s">
-        <v>1545</v>
+    <row r="61" spans="1:13" ht="67.5">
+      <c r="A61" s="10" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>1532</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>1544</v>
+        <v>28</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>12</v>
@@ -15030,14 +15060,11 @@
     <row r="62" spans="1:13" ht="31.5" customHeight="1">
       <c r="A62" s="10"/>
       <c r="B62" s="11"/>
-      <c r="E62" s="9" t="s">
-        <v>1541</v>
-      </c>
       <c r="F62" s="9" t="s">
-        <v>1535</v>
+        <v>25</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H62" s="9">
         <v>32</v>
@@ -15052,19 +15079,19 @@
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="E63" s="9" t="s">
+        <v>1543</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>1542</v>
       </c>
-      <c r="F63" s="9" t="s">
-        <v>1536</v>
-      </c>
       <c r="G63" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H63" s="9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>1537</v>
+        <v>13</v>
       </c>
       <c r="J63" s="9"/>
       <c r="M63" s="14"/>
@@ -15073,19 +15100,19 @@
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="E64" s="9" t="s">
-        <v>1543</v>
+        <v>1539</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="G64" s="9" t="s">
         <v>113</v>
       </c>
       <c r="H64" s="9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>1537</v>
+        <v>13</v>
       </c>
       <c r="J64" s="9"/>
       <c r="M64" s="14"/>
@@ -15093,20 +15120,20 @@
     <row r="65" spans="1:13" ht="31.5" customHeight="1">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
-      <c r="E65" s="12" t="s">
-        <v>1552</v>
+      <c r="E65" s="9" t="s">
+        <v>1540</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>1551</v>
+        <v>1534</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="H65" s="9">
         <v>8</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>17</v>
+        <v>1535</v>
       </c>
       <c r="J65" s="9"/>
       <c r="M65" s="14"/>
@@ -15114,17 +15141,20 @@
     <row r="66" spans="1:13" ht="31.5" customHeight="1">
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
+      <c r="E66" s="9" t="s">
+        <v>1541</v>
+      </c>
       <c r="F66" s="9" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="G66" s="9" t="s">
         <v>113</v>
       </c>
       <c r="H66" s="9">
-        <v>500</v>
+        <v>8</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="J66" s="9"/>
       <c r="M66" s="14"/>
@@ -15132,78 +15162,81 @@
     <row r="67" spans="1:13" ht="31.5" customHeight="1">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
+      <c r="E67" s="12" t="s">
+        <v>1550</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>1549</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="9">
+        <v>8</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="J67" s="9"/>
       <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13" ht="31.5" customHeight="1">
       <c r="A68" s="10"/>
       <c r="B68" s="11"/>
+      <c r="F68" s="9" t="s">
+        <v>1537</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H68" s="9">
+        <v>500</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>1538</v>
+      </c>
       <c r="J68" s="9"/>
       <c r="M68" s="14"/>
     </row>
-    <row r="69" spans="1:13" ht="54">
-      <c r="A69" s="10" t="s">
-        <v>1502</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>1503</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>1500</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H69" s="9">
-        <v>32</v>
-      </c>
-      <c r="I69" s="9" t="s">
-        <v>13</v>
-      </c>
+    <row r="69" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A69" s="10"/>
+      <c r="B69" s="11"/>
       <c r="J69" s="9"/>
       <c r="M69" s="14"/>
     </row>
     <row r="70" spans="1:13" ht="31.5" customHeight="1">
       <c r="A70" s="10"/>
       <c r="B70" s="11"/>
-      <c r="F70" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H70" s="9">
-        <v>32</v>
-      </c>
-      <c r="I70" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J70" s="9"/>
       <c r="M70" s="14"/>
     </row>
-    <row r="71" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A71" s="10"/>
-      <c r="B71" s="11"/>
+    <row r="71" spans="1:13" ht="54">
+      <c r="A71" s="10" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>1500</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="F71" s="9" t="s">
-        <v>1504</v>
+        <v>28</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>1477</v>
+        <v>12</v>
       </c>
       <c r="H71" s="9">
         <v>32</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>1478</v>
+        <v>13</v>
       </c>
       <c r="J71" s="9"/>
       <c r="M71" s="14"/>
@@ -15211,36 +15244,35 @@
     <row r="72" spans="1:13" ht="31.5" customHeight="1">
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
+      <c r="F72" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="9">
+        <v>32</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="J72" s="9"/>
       <c r="M72" s="14"/>
     </row>
-    <row r="73" spans="1:13" ht="54">
-      <c r="A73" s="10" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>1530</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>84</v>
-      </c>
+    <row r="73" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A73" s="10"/>
+      <c r="B73" s="11"/>
       <c r="F73" s="9" t="s">
-        <v>28</v>
+        <v>1504</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>12</v>
+        <v>1477</v>
       </c>
       <c r="H73" s="9">
         <v>32</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>13</v>
+        <v>1478</v>
       </c>
       <c r="J73" s="9"/>
       <c r="M73" s="14"/>
@@ -15248,38 +15280,36 @@
     <row r="74" spans="1:13" ht="31.5" customHeight="1">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
-      <c r="F74" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" s="9">
-        <v>32</v>
-      </c>
-      <c r="I74" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J74" s="9"/>
       <c r="M74" s="14"/>
     </row>
-    <row r="75" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A75" s="10"/>
-      <c r="B75" s="11"/>
-      <c r="E75" s="9" t="s">
-        <v>1545</v>
+    <row r="75" spans="1:13" ht="54">
+      <c r="A75" s="10" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>1504</v>
+        <v>28</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H75" s="9">
         <v>32</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="J75" s="9"/>
       <c r="M75" s="14"/>
@@ -15287,23 +15317,17 @@
     <row r="76" spans="1:13" ht="31.5" customHeight="1">
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
-      <c r="D76" s="12" t="s">
-        <v>1554</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>1532</v>
-      </c>
       <c r="F76" s="9" t="s">
-        <v>1531</v>
+        <v>25</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H76" s="9">
         <v>32</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="J76" s="9"/>
       <c r="M76" s="14"/>
@@ -15311,36 +15335,44 @@
     <row r="77" spans="1:13" ht="31.5" customHeight="1">
       <c r="A77" s="10"/>
       <c r="B77" s="11"/>
+      <c r="E77" s="9" t="s">
+        <v>1543</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" s="9">
+        <v>32</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="J77" s="9"/>
       <c r="M77" s="14"/>
     </row>
-    <row r="78" spans="1:13" ht="54">
-      <c r="A78" s="10" t="s">
-        <v>1499</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>1501</v>
-      </c>
+    <row r="78" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A78" s="10"/>
+      <c r="B78" s="11"/>
       <c r="D78" s="12" t="s">
-        <v>1500</v>
-      </c>
-      <c r="E78" s="13" t="s">
-        <v>84</v>
+        <v>1552</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>1530</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>28</v>
+        <v>1529</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="H78" s="9">
         <v>32</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="J78" s="9"/>
       <c r="M78" s="14"/>
@@ -15348,38 +15380,36 @@
     <row r="79" spans="1:13" ht="31.5" customHeight="1">
       <c r="A79" s="10"/>
       <c r="B79" s="11"/>
-      <c r="F79" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H79" s="9">
-        <v>32</v>
-      </c>
-      <c r="I79" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J79" s="9"/>
       <c r="M79" s="14"/>
     </row>
-    <row r="80" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A80" s="10"/>
-      <c r="B80" s="11"/>
-      <c r="E80" s="9" t="s">
-        <v>1545</v>
+    <row r="80" spans="1:13" ht="54">
+      <c r="A80" s="10" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>1500</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>1504</v>
+        <v>28</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>1477</v>
+        <v>12</v>
       </c>
       <c r="H80" s="9">
         <v>32</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>1478</v>
+        <v>13</v>
       </c>
       <c r="J80" s="9"/>
       <c r="M80" s="14"/>
@@ -15387,11 +15417,8 @@
     <row r="81" spans="1:13" ht="31.5" customHeight="1">
       <c r="A81" s="10"/>
       <c r="B81" s="11"/>
-      <c r="E81" s="9" t="s">
-        <v>1550</v>
-      </c>
-      <c r="F81" s="139" t="s">
-        <v>1549</v>
+      <c r="F81" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="G81" s="9" t="s">
         <v>12</v>
@@ -15399,8 +15426,8 @@
       <c r="H81" s="9">
         <v>32</v>
       </c>
-      <c r="I81" s="139" t="s">
-        <v>1553</v>
+      <c r="I81" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="J81" s="9"/>
       <c r="M81" s="14"/>
@@ -15409,19 +15436,19 @@
       <c r="A82" s="10"/>
       <c r="B82" s="11"/>
       <c r="E82" s="9" t="s">
-        <v>1481</v>
+        <v>1543</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>1476</v>
+        <v>1504</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>1477</v>
       </c>
       <c r="H82" s="9">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>1505</v>
+        <v>1478</v>
       </c>
       <c r="J82" s="9"/>
       <c r="M82" s="14"/>
@@ -15430,19 +15457,19 @@
       <c r="A83" s="10"/>
       <c r="B83" s="11"/>
       <c r="E83" s="9" t="s">
-        <v>1480</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>1479</v>
+        <v>1548</v>
+      </c>
+      <c r="F83" s="139" t="s">
+        <v>1547</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H83" s="9">
         <v>32</v>
       </c>
-      <c r="I83" s="9" t="s">
-        <v>1505</v>
+      <c r="I83" s="139" t="s">
+        <v>1551</v>
       </c>
       <c r="J83" s="9"/>
       <c r="M83" s="14"/>
@@ -15451,16 +15478,16 @@
       <c r="A84" s="10"/>
       <c r="B84" s="11"/>
       <c r="E84" s="9" t="s">
-        <v>1514</v>
+        <v>1481</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>1497</v>
+        <v>1476</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>16</v>
+        <v>1477</v>
       </c>
       <c r="H84" s="9">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>1505</v>
@@ -15471,11 +15498,11 @@
     <row r="85" spans="1:13" ht="31.5" customHeight="1">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
-      <c r="E85" s="12" t="s">
-        <v>1482</v>
+      <c r="E85" s="9" t="s">
+        <v>1480</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>1508</v>
+        <v>1479</v>
       </c>
       <c r="G85" s="9" t="s">
         <v>16</v>
@@ -15493,16 +15520,16 @@
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="E86" s="9" t="s">
-        <v>1484</v>
+        <v>1514</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>1483</v>
+        <v>1497</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>1477</v>
+        <v>16</v>
       </c>
       <c r="H86" s="9">
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="I86" s="9" t="s">
         <v>1505</v>
@@ -15513,17 +15540,17 @@
     <row r="87" spans="1:13" ht="31.5" customHeight="1">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
-      <c r="E87" s="9" t="s">
-        <v>1486</v>
+      <c r="E87" s="12" t="s">
+        <v>1482</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>1485</v>
+        <v>1508</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>1477</v>
+        <v>16</v>
       </c>
       <c r="H87" s="9">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I87" s="9" t="s">
         <v>1505</v>
@@ -15535,16 +15562,16 @@
       <c r="A88" s="10"/>
       <c r="B88" s="11"/>
       <c r="E88" s="9" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>1489</v>
+        <v>1477</v>
       </c>
       <c r="H88" s="9">
-        <v>64</v>
+        <v>500</v>
       </c>
       <c r="I88" s="9" t="s">
         <v>1505</v>
@@ -15556,10 +15583,10 @@
       <c r="A89" s="10"/>
       <c r="B89" s="11"/>
       <c r="E89" s="9" t="s">
-        <v>1495</v>
+        <v>1486</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>1493</v>
+        <v>1485</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>1477</v>
@@ -15568,7 +15595,7 @@
         <v>200</v>
       </c>
       <c r="I89" s="9" t="s">
-        <v>1494</v>
+        <v>1505</v>
       </c>
       <c r="J89" s="9"/>
       <c r="M89" s="14"/>
@@ -15576,36 +15603,41 @@
     <row r="90" spans="1:13" ht="31.5" customHeight="1">
       <c r="A90" s="10"/>
       <c r="B90" s="11"/>
+      <c r="E90" s="9" t="s">
+        <v>1487</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>1488</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H90" s="9">
+        <v>64</v>
+      </c>
+      <c r="I90" s="9" t="s">
+        <v>1505</v>
+      </c>
       <c r="J90" s="9"/>
       <c r="M90" s="14"/>
     </row>
-    <row r="91" spans="1:13" ht="297">
-      <c r="A91" s="10" t="s">
-        <v>1506</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>1547</v>
+    <row r="91" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A91" s="10"/>
+      <c r="B91" s="11"/>
+      <c r="E91" s="9" t="s">
+        <v>1495</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>28</v>
+        <v>1493</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>12</v>
+        <v>1477</v>
       </c>
       <c r="H91" s="9">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="I91" s="9" t="s">
-        <v>13</v>
+        <v>1494</v>
       </c>
       <c r="J91" s="9"/>
       <c r="M91" s="14"/>
@@ -15613,35 +15645,36 @@
     <row r="92" spans="1:13" ht="31.5" customHeight="1">
       <c r="A92" s="10"/>
       <c r="B92" s="11"/>
-      <c r="F92" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G92" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H92" s="9">
-        <v>32</v>
-      </c>
-      <c r="I92" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J92" s="9"/>
       <c r="M92" s="14"/>
     </row>
-    <row r="93" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A93" s="10"/>
-      <c r="B93" s="11"/>
+    <row r="93" spans="1:13" ht="297">
+      <c r="A93" s="10" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>1545</v>
+      </c>
       <c r="F93" s="9" t="s">
-        <v>1504</v>
+        <v>28</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>1477</v>
+        <v>12</v>
       </c>
       <c r="H93" s="9">
         <v>32</v>
       </c>
       <c r="I93" s="9" t="s">
-        <v>1478</v>
+        <v>13</v>
       </c>
       <c r="J93" s="9"/>
       <c r="M93" s="14"/>
@@ -15649,36 +15682,35 @@
     <row r="94" spans="1:13" ht="31.5" customHeight="1">
       <c r="A94" s="10"/>
       <c r="B94" s="11"/>
+      <c r="F94" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H94" s="9">
+        <v>32</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="J94" s="9"/>
       <c r="M94" s="14"/>
     </row>
-    <row r="95" spans="1:13" ht="409.5">
-      <c r="A95" s="10" t="s">
-        <v>1509</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>1510</v>
-      </c>
-      <c r="D95" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>1548</v>
-      </c>
+    <row r="95" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A95" s="10"/>
+      <c r="B95" s="11"/>
       <c r="F95" s="9" t="s">
-        <v>28</v>
+        <v>1504</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>12</v>
+        <v>1477</v>
       </c>
       <c r="H95" s="9">
         <v>32</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>13</v>
+        <v>1478</v>
       </c>
       <c r="J95" s="9"/>
       <c r="M95" s="14"/>
@@ -15686,31 +15718,27 @@
     <row r="96" spans="1:13" ht="31.5" customHeight="1">
       <c r="A96" s="10"/>
       <c r="B96" s="11"/>
-      <c r="F96" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G96" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H96" s="9">
-        <v>32</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="J96" s="9"/>
       <c r="M96" s="14"/>
     </row>
-    <row r="97" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A97" s="137"/>
-      <c r="B97" s="138"/>
-      <c r="C97" s="139"/>
-      <c r="D97" s="139"/>
-      <c r="E97" s="9" t="s">
-        <v>1550</v>
-      </c>
-      <c r="F97" s="139" t="s">
-        <v>1549</v>
+    <row r="97" spans="1:13" ht="409.5">
+      <c r="A97" s="10" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="G97" s="9" t="s">
         <v>12</v>
@@ -15719,21 +15747,16 @@
         <v>32</v>
       </c>
       <c r="I97" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J97" s="139"/>
-      <c r="K97" s="139"/>
-      <c r="L97" s="139"/>
-      <c r="M97" s="141"/>
+        <v>13</v>
+      </c>
+      <c r="J97" s="9"/>
+      <c r="M97" s="14"/>
     </row>
     <row r="98" spans="1:13" ht="31.5" customHeight="1">
       <c r="A98" s="10"/>
       <c r="B98" s="11"/>
-      <c r="E98" s="9" t="s">
-        <v>1480</v>
-      </c>
       <c r="F98" s="9" t="s">
-        <v>1511</v>
+        <v>25</v>
       </c>
       <c r="G98" s="9" t="s">
         <v>12</v>
@@ -15742,46 +15765,53 @@
         <v>32</v>
       </c>
       <c r="I98" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J98" s="9"/>
       <c r="M98" s="14"/>
     </row>
     <row r="99" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A99" s="10"/>
-      <c r="B99" s="11"/>
+      <c r="A99" s="137"/>
+      <c r="B99" s="138"/>
+      <c r="C99" s="139"/>
+      <c r="D99" s="139"/>
       <c r="E99" s="9" t="s">
-        <v>1496</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>1497</v>
+        <v>1548</v>
+      </c>
+      <c r="F99" s="139" t="s">
+        <v>1547</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H99" s="9">
         <v>32</v>
       </c>
       <c r="I99" s="9" t="s">
-        <v>1505</v>
-      </c>
-      <c r="J99" s="9"/>
-      <c r="M99" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="J99" s="139"/>
+      <c r="K99" s="139"/>
+      <c r="L99" s="139"/>
+      <c r="M99" s="141"/>
     </row>
     <row r="100" spans="1:13" ht="31.5" customHeight="1">
       <c r="A100" s="10"/>
       <c r="B100" s="11"/>
+      <c r="E100" s="9" t="s">
+        <v>1480</v>
+      </c>
       <c r="F100" s="9" t="s">
-        <v>1485</v>
+        <v>1511</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>1477</v>
+        <v>12</v>
       </c>
       <c r="H100" s="9">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I100" s="9" t="s">
-        <v>1505</v>
+        <v>17</v>
       </c>
       <c r="J100" s="9"/>
       <c r="M100" s="14"/>
@@ -15789,14 +15819,17 @@
     <row r="101" spans="1:13" ht="31.5" customHeight="1">
       <c r="A101" s="10"/>
       <c r="B101" s="11"/>
+      <c r="E101" s="9" t="s">
+        <v>1496</v>
+      </c>
       <c r="F101" s="9" t="s">
-        <v>1488</v>
+        <v>1497</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>1489</v>
+        <v>16</v>
       </c>
       <c r="H101" s="9">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="I101" s="9" t="s">
         <v>1505</v>
@@ -15807,17 +15840,14 @@
     <row r="102" spans="1:13" ht="31.5" customHeight="1">
       <c r="A102" s="10"/>
       <c r="B102" s="11"/>
-      <c r="E102" s="9" t="s">
-        <v>1513</v>
-      </c>
       <c r="F102" s="9" t="s">
-        <v>1512</v>
+        <v>1485</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>16</v>
+        <v>1477</v>
       </c>
       <c r="H102" s="9">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="I102" s="9" t="s">
         <v>1505</v>
@@ -15829,16 +15859,16 @@
       <c r="A103" s="10"/>
       <c r="B103" s="11"/>
       <c r="F103" s="9" t="s">
-        <v>968</v>
+        <v>1488</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>12</v>
+        <v>1489</v>
       </c>
       <c r="H103" s="9">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>970</v>
+        <v>1505</v>
       </c>
       <c r="J103" s="9"/>
       <c r="M103" s="14"/>
@@ -15846,17 +15876,20 @@
     <row r="104" spans="1:13" ht="31.5" customHeight="1">
       <c r="A104" s="10"/>
       <c r="B104" s="11"/>
+      <c r="E104" s="9" t="s">
+        <v>1513</v>
+      </c>
       <c r="F104" s="9" t="s">
-        <v>969</v>
+        <v>1512</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H104" s="9">
         <v>32</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>877</v>
+        <v>1505</v>
       </c>
       <c r="J104" s="9"/>
       <c r="M104" s="14"/>
@@ -15865,16 +15898,16 @@
       <c r="A105" s="10"/>
       <c r="B105" s="11"/>
       <c r="F105" s="9" t="s">
-        <v>260</v>
+        <v>968</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="H105" s="9">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>17</v>
+        <v>970</v>
       </c>
       <c r="J105" s="9"/>
       <c r="M105" s="14"/>
@@ -15882,12 +15915,36 @@
     <row r="106" spans="1:13" ht="31.5" customHeight="1">
       <c r="A106" s="10"/>
       <c r="B106" s="11"/>
+      <c r="F106" s="9" t="s">
+        <v>969</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H106" s="9">
+        <v>32</v>
+      </c>
+      <c r="I106" s="9" t="s">
+        <v>877</v>
+      </c>
       <c r="J106" s="9"/>
       <c r="M106" s="14"/>
     </row>
     <row r="107" spans="1:13" ht="31.5" customHeight="1">
       <c r="A107" s="10"/>
       <c r="B107" s="11"/>
+      <c r="F107" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H107" s="9">
+        <v>4</v>
+      </c>
+      <c r="I107" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="J107" s="9"/>
       <c r="M107" s="14"/>
     </row>
@@ -15927,22 +15984,28 @@
       <c r="J113" s="9"/>
       <c r="M113" s="14"/>
     </row>
-    <row r="114" spans="1:13" ht="32.25" customHeight="1">
+    <row r="114" spans="1:13" ht="31.5" customHeight="1">
       <c r="A114" s="10"/>
-      <c r="B114" s="15"/>
+      <c r="B114" s="11"/>
       <c r="J114" s="9"/>
-    </row>
-    <row r="115" spans="1:13" ht="32.25" customHeight="1">
+      <c r="M114" s="14"/>
+    </row>
+    <row r="115" spans="1:13" ht="31.5" customHeight="1">
       <c r="A115" s="10"/>
-      <c r="B115" s="15"/>
+      <c r="B115" s="11"/>
       <c r="J115" s="9"/>
       <c r="M115" s="14"/>
     </row>
-    <row r="116" spans="1:13" ht="31.5" customHeight="1">
+    <row r="116" spans="1:13" ht="32.25" customHeight="1">
+      <c r="A116" s="10"/>
+      <c r="B116" s="15"/>
       <c r="J116" s="9"/>
     </row>
-    <row r="117" spans="1:13" ht="31.5" customHeight="1">
+    <row r="117" spans="1:13" ht="32.25" customHeight="1">
+      <c r="A117" s="10"/>
+      <c r="B117" s="15"/>
       <c r="J117" s="9"/>
+      <c r="M117" s="14"/>
     </row>
     <row r="118" spans="1:13" ht="31.5" customHeight="1">
       <c r="J118" s="9"/>
@@ -15982,6 +16045,12 @@
     </row>
     <row r="130" spans="10:10" ht="31.5" customHeight="1">
       <c r="J130" s="9"/>
+    </row>
+    <row r="131" spans="10:10" ht="31.5" customHeight="1">
+      <c r="J131" s="9"/>
+    </row>
+    <row r="132" spans="10:10" ht="31.5" customHeight="1">
+      <c r="J132" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -16246,7 +16315,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -16468,9 +16537,15 @@
       <c r="C12" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="D12" s="80"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="7"/>
+      <c r="D12" s="80" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E12" s="93">
+        <v>3320</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>1555</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="42" customHeight="1">
       <c r="A13" s="151"/>
@@ -16910,8 +16985,8 @@
   <dimension ref="A1:M258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17003,7 +17078,7 @@
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="E3" s="9" t="s">
-        <v>1303</v>
+        <v>1553</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>1300</v>
@@ -20766,7 +20841,7 @@
   <dimension ref="A1:M214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>

</xml_diff>